<commit_message>
Added a few epic items to ALLITEMS File, made Common Walkie Talkie data the same across all files.
</commit_message>
<xml_diff>
--- a/BidBattlesGemAuctions.xlsx
+++ b/BidBattlesGemAuctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/544eb1111fb4475e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="597" documentId="8_{D149EF83-8D04-4C49-A013-BE601F3CE8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1910B44B-758F-44BA-8CA8-D283F1692068}"/>
+  <xr:revisionPtr revIDLastSave="598" documentId="8_{D149EF83-8D04-4C49-A013-BE601F3CE8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B1E3AE5-EA12-4A3C-A833-26371B99A79F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B7B61ADF-0F24-4110-B604-A0DDBCD9C6AE}"/>
   </bookViews>
@@ -631,9 +631,6 @@
     <t>Duke of the Federation</t>
   </si>
   <si>
-    <t>Leaning Tower of Pisa?</t>
-  </si>
-  <si>
     <t>Pyramid</t>
   </si>
   <si>
@@ -677,6 +674,9 @@
   </si>
   <si>
     <t>Stone Portal</t>
+  </si>
+  <si>
+    <t>Leaning Tower Of Pisa</t>
   </si>
 </sst>
 </file>
@@ -3620,7 +3620,7 @@
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
         <v>111</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="24" spans="1:8" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>55</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
@@ -3978,7 +3978,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
@@ -4040,7 +4040,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" t="s">
         <v>55</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B33" t="s">
         <v>55</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34" t="s">
         <v>55</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>55</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s">
         <v>55</v>
@@ -4229,7 +4229,7 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>55</v>
@@ -4245,7 +4245,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B44" t="s">
         <v>55</v>
@@ -4590,7 +4590,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
@@ -6682,13 +6682,13 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B176" s="1"/>
     </row>
     <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B177" t="s">
         <v>0</v>
@@ -6819,7 +6819,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>

</xml_diff>